<commit_message>
Adding new sunburst visualizations
</commit_message>
<xml_diff>
--- a/untl-bs/data/3_SpreadVs.Usage/ForSunburstChart.xlsx
+++ b/untl-bs/data/3_SpreadVs.Usage/ForSunburstChart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\Documents\GitHub\portal-leading\untl-bs\data\3_SpreadVs.Usage\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hjones\Documents\GitHub\portal-leading\untl-bs\data\3_SpreadVs.Usage\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06EF1E48-6F8B-441F-9888-3A688AFDD2CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E664A8D-277E-491A-9325-635C989385B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2AF4E2AB-D538-4D02-A969-46AACDD51A95}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{2AF4E2AB-D538-4D02-A969-46AACDD51A95}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="7" r:id="rId1"/>
@@ -20,10 +20,32 @@
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">'2-layers'!$B$2:$C$212</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">'2-layers'!$D$1</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'3-layers'!$E$510:$E$577</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'3-layers'!$B$2:$D$623</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'3-layers'!$E$1</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'3-layers'!$E$2:$E$623</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'3-layers'!$C$510:$D$577</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'3-layers'!$E$510:$E$577</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'3-layers'!$C$510:$D$577</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'3-layers'!$E$510:$E$577</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'3-layers'!$C$61:$D$81</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">'3-layers'!$E$61:$E$81</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">'2-layers'!$D$2:$D$212</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'3-layers'!$B$2:$D$623</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'3-layers'!$E$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'3-layers'!$E$2:$E$623</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">'3-layers'!$C$273:$D$303</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">'3-layers'!$E$273:$E$303</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">'3-layers'!$C$510:$D$577</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">'3-layers'!$E$510:$E$577</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">'3-layers'!$C$510:$D$577</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">'3-layers'!$E$510:$E$577</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">'3-layers'!$C$510:$D$577</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">'3-layers'!$E$510:$E$577</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'3-layers'!$C$510:$D$577</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'3-layers'!$E$510:$E$577</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'3-layers'!$C$273:$D$303</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'3-layers'!$E$273:$E$303</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'3-layers'!$C$47:$D$60</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'3-layers'!$E$47:$E$60</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'3-layers'!$C$510:$D$577</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,10 +57,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -4250,10 +4272,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.11</cx:f>
       </cx:strDim>
       <cx:numDim type="size">
-        <cx:f>_xlchart.v1.5</cx:f>
+        <cx:f>_xlchart.v1.13</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -4346,7 +4368,7 @@
         <cx:series layoutId="sunburst" uniqueId="{C9AAD9EF-8EFB-4A2C-BD21-B2D3CC18493D}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.4</cx:f>
+              <cx:f>_xlchart.v1.12</cx:f>
               <cx:v>OccurrenceCount</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4357,6 +4379,232 @@
         </cx:series>
       </cx:plotAreaRegion>
     </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx3.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.7</cx:f>
+      </cx:strDim>
+      <cx:numDim type="size">
+        <cx:f>_xlchart.v1.8</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>"Architecture" Branch, UNTL-BS</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>"Architecture" Branch, UNTL-BS</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="sunburst" uniqueId="{55C5441D-12D4-4764-B058-8197F840DC0B}">
+          <cx:dataLabels pos="ctr">
+            <cx:visibility seriesName="0" categoryName="1" value="1"/>
+            <cx:separator>, </cx:separator>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx4.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.18</cx:f>
+      </cx:strDim>
+      <cx:numDim type="size">
+        <cx:f>_xlchart.v1.19</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>"Arts and Crafts" Branch, UNTL-BS</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>"Arts and Crafts" Branch, UNTL-BS</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="sunburst" uniqueId="{47F740FF-D589-461C-A71D-5129F81AE146}">
+          <cx:dataLabels pos="ctr">
+            <cx:visibility seriesName="0" categoryName="1" value="1"/>
+            <cx:separator>, </cx:separator>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+    <cx:legend pos="r" align="ctr" overlay="0"/>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx5.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.9</cx:f>
+      </cx:strDim>
+      <cx:numDim type="size">
+        <cx:f>_xlchart.v1.10</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>"Social Life and Customs" Branch, UNTL-BS</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>"Social Life and Customs" Branch, UNTL-BS</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="sunburst" uniqueId="{21EE0D18-30DE-4130-A35F-ED671646679E}">
+          <cx:dataLabels pos="ctr">
+            <cx:visibility seriesName="0" categoryName="1" value="1"/>
+            <cx:separator>, </cx:separator>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx6.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.20</cx:f>
+      </cx:strDim>
+      <cx:numDim type="size">
+        <cx:f>_xlchart.v1.21</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>"Ladscape and Nature" Branch, UNTL-BS</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>"Ladscape and Nature" Branch, UNTL-BS</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="sunburst" uniqueId="{25CAEACD-E56E-4DD2-85F3-C683F373470C}">
+          <cx:dataLabels pos="ctr">
+            <cx:visibility seriesName="0" categoryName="1" value="1"/>
+            <cx:separator>, </cx:separator>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+    <cx:legend pos="r" align="ctr" overlay="0"/>
   </cx:chart>
 </cx:chartSpace>
 </file>
@@ -4402,6 +4650,166 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4952,6 +5360,2046 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="381">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="381">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="381">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="381">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="381">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6191,6 +8639,318 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>212912</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>179294</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>163607</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>89641</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Chart 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0069BBDC-9F6B-4265-BA39-B7F7D228A653}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13559118" y="7037294"/>
+              <a:ext cx="7817224" cy="7911347"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>96115</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>176646</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>391391</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>167121</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="6" name="Chart 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B12355D-EAFB-4CD8-87AB-0D06DBF47C72}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="24965024" y="1510146"/>
+              <a:ext cx="7568912" cy="5705475"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>313765</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>25468</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>353673</xdr:colOff>
+      <xdr:row>124</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="12" name="Chart 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A27B28D4-8282-4252-9C51-F3922C48D971}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="15475324" y="15455968"/>
+              <a:ext cx="7906437" cy="8210856"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>119063</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>90488</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="13" name="Chart 12">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B608F0A3-8D81-4F66-B115-83AAB3F3F935}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="25565100" y="8001000"/>
+              <a:ext cx="6824663" cy="5805488"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>This chart isn't available in your version of Excel.
+Editing this shape or saving this workbook into a different file format will permanently break the chart.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6493,8 +9253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{971BFE19-4057-4825-B56C-9D04B1D1272C}">
   <dimension ref="A1:G999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1048576"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54:F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19495,8 +22255,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{112CCAD9-9EE7-459D-B0D7-D739A70D61C6}">
   <dimension ref="A1:E705"/>
   <sheetViews>
-    <sheetView topLeftCell="D19" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24006,7 +26766,7 @@
       <c r="A705"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E212">
+  <sortState ref="A2:E212">
     <sortCondition ref="A2:A212"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -24019,8 +26779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E7B804A-BFE3-489B-94E1-6E19A4EA249A}">
   <dimension ref="A1:F625"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="G76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I107" sqref="I107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33020,7 +35780,7 @@
     </row>
     <row r="625" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L1008">
+  <sortState ref="A2:L1008">
     <sortCondition ref="A2:A1008"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>